<commit_message>
update chapter03 and requirements
</commit_message>
<xml_diff>
--- a/chapter03/notebooks/results.xlsx
+++ b/chapter03/notebooks/results.xlsx
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>149.52</v>
+        <v>149.38</v>
       </c>
       <c r="F2" t="n">
-        <v>24245.44</v>
+        <v>24237.06</v>
       </c>
       <c r="G2" t="n">
-        <v>155.71</v>
+        <v>155.68</v>
       </c>
     </row>
     <row r="3">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>16.13</v>
+        <v>16.28</v>
       </c>
       <c r="F4" t="n">
-        <v>403.41</v>
+        <v>411.96</v>
       </c>
       <c r="G4" t="n">
-        <v>20.09</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="5">
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>148.57</v>
+        <v>150.73</v>
       </c>
       <c r="F5" t="n">
-        <v>23929.2</v>
+        <v>24673.77</v>
       </c>
       <c r="G5" t="n">
-        <v>154.69</v>
+        <v>157.08</v>
       </c>
     </row>
     <row r="6">
@@ -630,13 +630,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>16.18</v>
+        <v>16.21</v>
       </c>
       <c r="F7" t="n">
-        <v>405.84</v>
+        <v>409.55</v>
       </c>
       <c r="G7" t="n">
-        <v>20.15</v>
+        <v>20.24</v>
       </c>
     </row>
     <row r="8">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>147.92</v>
+        <v>150.68</v>
       </c>
       <c r="F8" t="n">
-        <v>23724.62</v>
+        <v>24659.81</v>
       </c>
       <c r="G8" t="n">
-        <v>154.03</v>
+        <v>157.03</v>
       </c>
     </row>
     <row r="9">
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>16.11</v>
+        <v>16.24</v>
       </c>
       <c r="F10" t="n">
-        <v>404.87</v>
+        <v>409</v>
       </c>
       <c r="G10" t="n">
-        <v>20.12</v>
+        <v>20.22</v>
       </c>
     </row>
     <row r="11">
@@ -746,13 +746,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>30.42</v>
+        <v>30.21</v>
       </c>
       <c r="F11" t="n">
-        <v>1383.1</v>
+        <v>1403.75</v>
       </c>
       <c r="G11" t="n">
-        <v>37.19</v>
+        <v>37.47</v>
       </c>
     </row>
     <row r="12">
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>26.14</v>
+        <v>26.3</v>
       </c>
       <c r="F13" t="n">
-        <v>1045.21</v>
+        <v>1021</v>
       </c>
       <c r="G13" t="n">
-        <v>32.33</v>
+        <v>31.95</v>
       </c>
     </row>
     <row r="14">
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>30.24</v>
+        <v>30.28</v>
       </c>
       <c r="F14" t="n">
-        <v>1399.92</v>
+        <v>1415.19</v>
       </c>
       <c r="G14" t="n">
-        <v>37.42</v>
+        <v>37.62</v>
       </c>
     </row>
     <row r="15">
@@ -891,13 +891,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>25.97</v>
+        <v>26.19</v>
       </c>
       <c r="F16" t="n">
-        <v>1037.33</v>
+        <v>1060.89</v>
       </c>
       <c r="G16" t="n">
-        <v>32.21</v>
+        <v>32.57</v>
       </c>
     </row>
     <row r="17">
@@ -920,13 +920,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>30.2</v>
+        <v>30.34</v>
       </c>
       <c r="F17" t="n">
-        <v>1406.6</v>
+        <v>1426.6</v>
       </c>
       <c r="G17" t="n">
-        <v>37.5</v>
+        <v>37.77</v>
       </c>
     </row>
     <row r="18">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>25.79</v>
+        <v>25.69</v>
       </c>
       <c r="F19" t="n">
-        <v>1027.56</v>
+        <v>1012.45</v>
       </c>
       <c r="G19" t="n">
-        <v>32.06</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="20">
@@ -1007,13 +1007,13 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>4.83</v>
+        <v>4.85</v>
       </c>
       <c r="F20" t="n">
-        <v>25.7</v>
+        <v>34.2</v>
       </c>
       <c r="G20" t="n">
-        <v>5.07</v>
+        <v>5.85</v>
       </c>
     </row>
     <row r="21">
@@ -1068,10 +1068,10 @@
         <v>4.83</v>
       </c>
       <c r="F22" t="n">
-        <v>26.97</v>
+        <v>26.48</v>
       </c>
       <c r="G22" t="n">
-        <v>5.19</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="23">
@@ -1097,10 +1097,10 @@
         <v>4.83</v>
       </c>
       <c r="F23" t="n">
-        <v>27.44</v>
+        <v>25.75</v>
       </c>
       <c r="G23" t="n">
-        <v>5.24</v>
+        <v>5.07</v>
       </c>
     </row>
     <row r="24">
@@ -1155,10 +1155,10 @@
         <v>4.83</v>
       </c>
       <c r="F25" t="n">
-        <v>24.95</v>
+        <v>28.64</v>
       </c>
       <c r="G25" t="n">
-        <v>4.99</v>
+        <v>5.35</v>
       </c>
     </row>
     <row r="26">
@@ -1181,13 +1181,13 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4.83</v>
       </c>
       <c r="F26" t="n">
-        <v>35.31</v>
+        <v>25.8</v>
       </c>
       <c r="G26" t="n">
-        <v>5.94</v>
+        <v>5.08</v>
       </c>
     </row>
     <row r="27">
@@ -1242,10 +1242,10 @@
         <v>4.83</v>
       </c>
       <c r="F28" t="n">
-        <v>24.91</v>
+        <v>31.61</v>
       </c>
       <c r="G28" t="n">
-        <v>4.99</v>
+        <v>5.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update polynomial regression and add docstrings
</commit_message>
<xml_diff>
--- a/chapter03/notebooks/results.xlsx
+++ b/chapter03/notebooks/results.xlsx
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>149.38</v>
+        <v>149.98</v>
       </c>
       <c r="F2" t="n">
-        <v>24237.06</v>
+        <v>24406.17</v>
       </c>
       <c r="G2" t="n">
-        <v>155.68</v>
+        <v>156.22</v>
       </c>
     </row>
     <row r="3">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>16.28</v>
+        <v>16.19</v>
       </c>
       <c r="F4" t="n">
-        <v>411.96</v>
+        <v>410.19</v>
       </c>
       <c r="G4" t="n">
-        <v>20.3</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="5">
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>150.73</v>
+        <v>149.3</v>
       </c>
       <c r="F5" t="n">
-        <v>24673.77</v>
+        <v>24187.04</v>
       </c>
       <c r="G5" t="n">
-        <v>157.08</v>
+        <v>155.52</v>
       </c>
     </row>
     <row r="6">
@@ -630,13 +630,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>16.21</v>
+        <v>16.11</v>
       </c>
       <c r="F7" t="n">
-        <v>409.55</v>
+        <v>402.52</v>
       </c>
       <c r="G7" t="n">
-        <v>20.24</v>
+        <v>20.06</v>
       </c>
     </row>
     <row r="8">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>150.68</v>
+        <v>148.91</v>
       </c>
       <c r="F8" t="n">
-        <v>24659.81</v>
+        <v>24070.94</v>
       </c>
       <c r="G8" t="n">
-        <v>157.03</v>
+        <v>155.15</v>
       </c>
     </row>
     <row r="9">
@@ -717,13 +717,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>16.24</v>
+        <v>15.92</v>
       </c>
       <c r="F10" t="n">
-        <v>409</v>
+        <v>394.06</v>
       </c>
       <c r="G10" t="n">
-        <v>20.22</v>
+        <v>19.85</v>
       </c>
     </row>
     <row r="11">
@@ -746,13 +746,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>30.21</v>
+        <v>30.63</v>
       </c>
       <c r="F11" t="n">
-        <v>1403.75</v>
+        <v>1422.76</v>
       </c>
       <c r="G11" t="n">
-        <v>37.47</v>
+        <v>37.72</v>
       </c>
     </row>
     <row r="12">
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>26.3</v>
+        <v>26.22</v>
       </c>
       <c r="F13" t="n">
-        <v>1021</v>
+        <v>1016.83</v>
       </c>
       <c r="G13" t="n">
-        <v>31.95</v>
+        <v>31.89</v>
       </c>
     </row>
     <row r="14">
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>30.28</v>
+        <v>30.39</v>
       </c>
       <c r="F14" t="n">
-        <v>1415.19</v>
+        <v>1382.76</v>
       </c>
       <c r="G14" t="n">
-        <v>37.62</v>
+        <v>37.19</v>
       </c>
     </row>
     <row r="15">
@@ -891,13 +891,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>26.19</v>
+        <v>25.72</v>
       </c>
       <c r="F16" t="n">
-        <v>1060.89</v>
+        <v>1018.61</v>
       </c>
       <c r="G16" t="n">
-        <v>32.57</v>
+        <v>31.92</v>
       </c>
     </row>
     <row r="17">
@@ -920,13 +920,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>30.34</v>
+        <v>30.4</v>
       </c>
       <c r="F17" t="n">
-        <v>1426.6</v>
+        <v>1404.37</v>
       </c>
       <c r="G17" t="n">
-        <v>37.77</v>
+        <v>37.47</v>
       </c>
     </row>
     <row r="18">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>25.69</v>
+        <v>25.94</v>
       </c>
       <c r="F19" t="n">
-        <v>1012.45</v>
+        <v>1008.05</v>
       </c>
       <c r="G19" t="n">
-        <v>31.82</v>
+        <v>31.75</v>
       </c>
     </row>
     <row r="20">
@@ -1007,13 +1007,13 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>4.85</v>
+        <v>4.83</v>
       </c>
       <c r="F20" t="n">
-        <v>34.2</v>
+        <v>24.96</v>
       </c>
       <c r="G20" t="n">
-        <v>5.85</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -1068,10 +1068,10 @@
         <v>4.83</v>
       </c>
       <c r="F22" t="n">
-        <v>26.48</v>
+        <v>32.72</v>
       </c>
       <c r="G22" t="n">
-        <v>5.15</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="23">
@@ -1097,10 +1097,10 @@
         <v>4.83</v>
       </c>
       <c r="F23" t="n">
-        <v>25.75</v>
+        <v>30.52</v>
       </c>
       <c r="G23" t="n">
-        <v>5.07</v>
+        <v>5.52</v>
       </c>
     </row>
     <row r="24">
@@ -1155,10 +1155,10 @@
         <v>4.83</v>
       </c>
       <c r="F25" t="n">
-        <v>28.64</v>
+        <v>30.23</v>
       </c>
       <c r="G25" t="n">
-        <v>5.35</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="26">
@@ -1184,10 +1184,10 @@
         <v>4.83</v>
       </c>
       <c r="F26" t="n">
-        <v>25.8</v>
+        <v>31.8</v>
       </c>
       <c r="G26" t="n">
-        <v>5.08</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="27">
@@ -1239,13 +1239,13 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>4.83</v>
+        <v>5.2</v>
       </c>
       <c r="F28" t="n">
-        <v>31.61</v>
+        <v>37.21</v>
       </c>
       <c r="G28" t="n">
-        <v>5.62</v>
+        <v>6.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>